<commit_message>
Added Time Results from my computer
Added my time results and a screen shot pic of my computer info
</commit_message>
<xml_diff>
--- a/RESULTS/Result.xlsx
+++ b/RESULTS/Result.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="21075" windowHeight="8775"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Result2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>Method</t>
   </si>
@@ -53,13 +53,16 @@
   </si>
   <si>
     <t>Avg Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREG </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +377,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -537,9 +546,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -595,6 +607,51 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>166686</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>301624</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>157232</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9707561" y="2476500"/>
+          <a:ext cx="4413251" cy="2443232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,7 +729,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -707,7 +763,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -883,14 +938,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
@@ -902,7 +957,7 @@
     <col min="8" max="8" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -928,7 +983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -949,7 +1004,7 @@
         <v>6.7383399999999996E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -970,7 +1025,7 @@
         <v>1.2696300000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -991,7 +1046,7 @@
         <v>1.36732E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1067,7 @@
         <v>3.22292E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1026,7 +1081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1040,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1054,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1068,7 +1123,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1082,8 +1137,153 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>3.3003299999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>3.1003099999999999E-2</v>
+      </c>
+      <c r="G16">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="H16">
+        <f>AVERAGE(E16:G16)</f>
+        <v>3.2335466666666667E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>0.83084000000000002</v>
+      </c>
+      <c r="C17">
+        <v>0.899733</v>
+      </c>
+      <c r="D17">
+        <v>0.90097499999999997</v>
+      </c>
+      <c r="E17">
+        <v>8.0008000000000006E-3</v>
+      </c>
+      <c r="F17">
+        <v>7.0007000000000003E-3</v>
+      </c>
+      <c r="G17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ref="H17:H19" si="1">AVERAGE(E17:G17)</f>
+        <v>7.3338333333333337E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>76</v>
+      </c>
+      <c r="C18">
+        <v>78</v>
+      </c>
+      <c r="D18">
+        <v>77</v>
+      </c>
+      <c r="E18">
+        <v>9.0008999999999992E-3</v>
+      </c>
+      <c r="F18">
+        <v>9.0008999999999992E-3</v>
+      </c>
+      <c r="G18">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>8.6672666666666662E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>64</v>
+      </c>
+      <c r="E19">
+        <v>4.0003999999999998E-2</v>
+      </c>
+      <c r="F19">
+        <v>3.9003900000000001E-2</v>
+      </c>
+      <c r="G19">
+        <v>3.9E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>3.9335966666666666E-2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:C14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>